<commit_message>
entity components and battle modules
</commit_message>
<xml_diff>
--- a/StaticData/Entity.xlsx
+++ b/StaticData/Entity.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\MonMoose\StaticData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\MonMoose\StaticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3851581C-E753-4421-9F9F-3F7A00859D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -108,18 +107,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Actor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RefId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,11 +445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -493,7 +492,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -538,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -552,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>